<commit_message>
Added standard deviation calculation
</commit_message>
<xml_diff>
--- a/ProjectData.xlsx
+++ b/ProjectData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusjo\Documents\Homework\Dependable Systems\DS_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD5F484-E822-403C-AB09-DC86A6FFAB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE140C9F-BB87-4CD9-9BCD-7564DFA1694B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26850" yWindow="13740" windowWidth="21600" windowHeight="11385" xr2:uid="{3C336683-77FF-48A0-A7D6-833CDC8D03F7}"/>
+    <workbookView xWindow="-28920" yWindow="11670" windowWidth="29040" windowHeight="15840" xr2:uid="{3C336683-77FF-48A0-A7D6-833CDC8D03F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>sqrt</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>C++</t>
+  </si>
+  <si>
+    <t>stdev</t>
   </si>
 </sst>
 </file>
@@ -1537,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53458342-0C7D-4471-9195-1FAB4E98B0A0}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,19 +1692,19 @@
         <v>15</v>
       </c>
       <c r="J5">
-        <f>D14</f>
+        <f>D15</f>
         <v>193.4</v>
       </c>
       <c r="K5">
-        <f>E14</f>
+        <f>E15</f>
         <v>84.2</v>
       </c>
       <c r="L5">
-        <f>F14</f>
+        <f>F15</f>
         <v>1713</v>
       </c>
       <c r="M5">
-        <f>G14</f>
+        <f>G15</f>
         <v>9.4</v>
       </c>
     </row>
@@ -1743,41 +1746,45 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>190</v>
-      </c>
-      <c r="E9">
-        <v>89</v>
-      </c>
-      <c r="F9">
-        <v>1713</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <f>_xlfn.STDEV.S(D2:D6)</f>
+        <v>19.651971911235776</v>
+      </c>
+      <c r="E8">
+        <f>_xlfn.STDEV.S(E2:E6)</f>
+        <v>6.6858058601787116</v>
+      </c>
+      <c r="F8">
+        <f>_xlfn.STDEV.S(F2:F6)</f>
+        <v>17.880156598866801</v>
+      </c>
+      <c r="G8">
+        <f>_xlfn.STDEV.S(G2:G6)</f>
+        <v>1.9493588689617958</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="E10">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F10">
-        <v>1693</v>
+        <v>1713</v>
       </c>
       <c r="G10">
         <v>8</v>
@@ -1785,74 +1792,112 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="E11">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="F11">
-        <v>1721</v>
+        <v>1693</v>
       </c>
       <c r="G11">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="E12">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F12">
-        <v>1716</v>
+        <v>1721</v>
       </c>
       <c r="G12">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E13">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="F13">
-        <v>1722</v>
+        <v>1716</v>
       </c>
       <c r="G13">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>196</v>
+      </c>
+      <c r="E14">
+        <v>71</v>
+      </c>
+      <c r="F14">
+        <v>1722</v>
+      </c>
+      <c r="G14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="D14">
-        <f>AVERAGE(D9:D13)</f>
+      <c r="D15">
+        <f>AVERAGE(D10:D14)</f>
         <v>193.4</v>
       </c>
-      <c r="E14">
-        <f>AVERAGE(E9:E13)</f>
+      <c r="E15">
+        <f>AVERAGE(E10:E14)</f>
         <v>84.2</v>
       </c>
-      <c r="F14">
-        <f>AVERAGE(F9:F13)</f>
+      <c r="F15">
+        <f>AVERAGE(F10:F14)</f>
         <v>1713</v>
       </c>
-      <c r="G14">
-        <f>AVERAGE(G9:G13)</f>
+      <c r="G15">
+        <f>AVERAGE(G10:G14)</f>
         <v>9.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <f>_xlfn.STDEV.S(D10:D14)</f>
+        <v>8.4734880657259435</v>
+      </c>
+      <c r="E16">
+        <f>_xlfn.STDEV.S(E10:E14)</f>
+        <v>8.5556998544829757</v>
+      </c>
+      <c r="F16">
+        <f>_xlfn.STDEV.S(F10:F14)</f>
+        <v>11.76860229593982</v>
+      </c>
+      <c r="G16">
+        <f>_xlfn.STDEV.S(G10:G14)</f>
+        <v>3.1304951684997051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>